<commit_message>
Ultimo Commit para sincronizar repositório local com GitHub
</commit_message>
<xml_diff>
--- a/Trabalhos/Fase4-Cap5/Dados.xlsx
+++ b/Trabalhos/Fase4-Cap5/Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Git\SmartCity_Hifive\Trabalhos\Fase4-Cap5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A318367-3D84-46EA-AB93-51883E82430E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883E9DE3-B7E1-4380-BA3D-527A0A131779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8205" yWindow="1710" windowWidth="20610" windowHeight="13395" xr2:uid="{251E3402-8D89-487D-9A56-B540A1F05287}"/>
+    <workbookView xWindow="41760" yWindow="2010" windowWidth="20610" windowHeight="13395" xr2:uid="{251E3402-8D89-487D-9A56-B540A1F05287}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="97">
   <si>
     <t>ID_USUARIO</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Isadora Portela</t>
   </si>
   <si>
-    <t>Mariana de Miranda</t>
-  </si>
-  <si>
     <t>Roberto Souza</t>
   </si>
   <si>
@@ -325,6 +322,12 @@
   </si>
   <si>
     <t>VL_DESCONTO PONTOS</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -767,25 +770,25 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
         <v>49</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>50</v>
-      </c>
-      <c r="I2" t="s">
-        <v>51</v>
       </c>
       <c r="J2" s="2">
         <v>31877</v>
@@ -802,25 +805,25 @@
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3">
         <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
         <v>49</v>
       </c>
-      <c r="H3" t="s">
-        <v>50</v>
-      </c>
       <c r="I3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J3" s="2">
         <v>32214</v>
@@ -837,25 +840,25 @@
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4">
         <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
         <v>49</v>
       </c>
-      <c r="H4" t="s">
-        <v>50</v>
-      </c>
       <c r="I4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J4" s="2">
         <v>34354</v>
@@ -872,25 +875,25 @@
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5">
         <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" t="s">
-        <v>50</v>
-      </c>
       <c r="I5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J5" s="2">
         <v>30489</v>
@@ -907,25 +910,25 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6">
         <v>556</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
         <v>49</v>
       </c>
-      <c r="H6" t="s">
-        <v>50</v>
-      </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J6" s="2">
         <v>35267</v>
@@ -942,25 +945,25 @@
         <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7">
         <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
         <v>49</v>
       </c>
-      <c r="H7" t="s">
-        <v>50</v>
-      </c>
       <c r="I7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J7" s="2">
         <v>38102</v>
@@ -977,25 +980,25 @@
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8">
         <v>785</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" t="s">
         <v>49</v>
       </c>
-      <c r="H8" t="s">
-        <v>50</v>
-      </c>
       <c r="I8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J8" s="2">
         <v>37146</v>
@@ -1012,25 +1015,25 @@
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9">
         <v>213</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" t="s">
         <v>49</v>
       </c>
-      <c r="H9" t="s">
-        <v>50</v>
-      </c>
       <c r="I9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J9" s="2">
         <v>36632</v>
@@ -1044,28 +1047,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10">
         <v>55</v>
       </c>
       <c r="F10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" t="s">
         <v>48</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>49</v>
       </c>
-      <c r="H10" t="s">
-        <v>50</v>
-      </c>
       <c r="I10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J10" s="2">
         <v>32339</v>
@@ -1079,28 +1082,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11">
         <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" t="s">
         <v>49</v>
       </c>
-      <c r="H11" t="s">
-        <v>50</v>
-      </c>
       <c r="I11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J11" s="2">
         <v>37236</v>
@@ -1130,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751FE93A-3FB8-4ECE-8947-C0614C4E1FBB}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,25 +1153,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>10</v>
@@ -1179,10 +1182,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2">
         <v>20</v>
@@ -1191,7 +1194,7 @@
         <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1205,10 +1208,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -1217,7 +1220,7 @@
         <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1231,10 +1234,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4">
         <v>15</v>
@@ -1243,7 +1246,7 @@
         <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1257,10 +1260,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5">
         <v>15</v>
@@ -1269,7 +1272,7 @@
         <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -1283,10 +1286,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6">
         <v>8</v>
@@ -1295,7 +1298,7 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -1309,10 +1312,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7">
         <v>12</v>
@@ -1321,7 +1324,7 @@
         <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -1335,10 +1338,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
         <v>82</v>
-      </c>
-      <c r="C8" t="s">
-        <v>83</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1347,7 +1350,7 @@
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G8">
         <v>4</v>
@@ -1361,10 +1364,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9">
         <v>22</v>
@@ -1373,7 +1376,7 @@
         <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G9">
         <v>5</v>
@@ -1387,10 +1390,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -1399,7 +1402,7 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G10">
         <v>5</v>
@@ -1413,10 +1416,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -1425,13 +1428,18 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G11">
         <v>4</v>
       </c>
       <c r="H11" s="2">
         <v>44657</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1444,7 +1452,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,22 +1467,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>